<commit_message>
Modif suivi & planning projet
</commit_message>
<xml_diff>
--- a/Gestion projet/planning_projet.xlsx
+++ b/Gestion projet/planning_projet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\stage\Stage_2025_ST_felixDL\Gestion projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBDD465-2348-4CFC-A417-9FE726887F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A75DF5A-0C7A-4FAF-9923-EBCBA0A81F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Réalisation du système</t>
   </si>
@@ -65,16 +65,49 @@
     <t>-</t>
   </si>
   <si>
-    <t>Mettre en place un environnement de travail</t>
-  </si>
-  <si>
     <t>Mettre en place une base de donnée</t>
   </si>
   <si>
-    <t>Mise en place des appareils</t>
-  </si>
-  <si>
     <t>Sélectionner un logiciel de développement adapté</t>
+  </si>
+  <si>
+    <t>Mise en place du matériel (ordinateur, afficheur, etc…)</t>
+  </si>
+  <si>
+    <t>Vérification matériel</t>
+  </si>
+  <si>
+    <t>Préparation de la fiche recette</t>
+  </si>
+  <si>
+    <t>Mettre en place l'interface</t>
+  </si>
+  <si>
+    <t>Coder le programme</t>
+  </si>
+  <si>
+    <t>Optimiser le code</t>
+  </si>
+  <si>
+    <t>Mettre en place son environnement de travail</t>
+  </si>
+  <si>
+    <t>Test de l'application (fonctionnement bouton, bdd, envoi trame, etc…) + correction si nécessaire</t>
+  </si>
+  <si>
+    <t>Réalisée</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Information potentiel</t>
+  </si>
+  <si>
+    <t>Réaliser le brouillon de l'algorithme</t>
+  </si>
+  <si>
+    <t>Communication entre les appareils</t>
   </si>
 </sst>
 </file>
@@ -124,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -132,11 +165,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -412,196 +462,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E22"/>
+  <dimension ref="B2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1">
-        <f>ROW(A1)</f>
+        <f>IF((D4&lt;&gt;""),ROW(C4)-3,"-")</f>
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
-        <f>ROW(A2)</f>
+        <f t="shared" ref="C5:C13" si="0">IF((D5&lt;&gt;""),ROW(C5)-3,"-")</f>
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
-        <f>ROW(A3)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
-        <f>ROW(A4)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="1">
-        <f t="shared" ref="C8:C10" si="0">ROW(A5)</f>
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="str">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="str">
         <f>C3</f>
         <v>Tâche n°</v>
       </c>
-      <c r="D12" s="2" t="str">
+      <c r="D15" s="4" t="str">
         <f>D3</f>
         <v>Nom de la tâche</v>
       </c>
-      <c r="E12" s="2" t="str">
-        <f t="shared" ref="E12" si="1">E3</f>
+      <c r="E15" s="2" t="str">
+        <f t="shared" ref="E15" si="1">E3</f>
         <v>Temps nécessaire (projection)</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <f>IF((D16&lt;&gt;""),ROW(A1),"-")</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <f>IF((D17&lt;&gt;""),ROW(A2),"-")</f>
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <f>IF((D18&lt;&gt;""),ROW(A3),"-")</f>
+        <v>3</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="1">
-        <f t="shared" ref="C14:C23" si="2">ROW(A2)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="1">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="1">
-        <f t="shared" si="2"/>
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <f>IF((D19&lt;&gt;""),ROW(A4),"-")</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="1">
-        <f t="shared" si="2"/>
+      <c r="D19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <f>IF((D20&lt;&gt;""),ROW(A5),"-")</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="1">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="1">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="1">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="1">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="1">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="D20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="str">
+        <f>IF((D21&lt;&gt;""),ROW(A6),"-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="str">
+        <f>IF((D22&lt;&gt;""),ROW(A8),"-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="str">
+        <f>IF((D23&lt;&gt;""),ROW(A9),"-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="str">
+        <f>IF((D24&lt;&gt;""),ROW(A10),"-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="str">
+        <f>IF((D25&lt;&gt;""),ROW(A11),"-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="str">
+        <f>IF((D26&lt;&gt;""),ROW(A12),"-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="str">
+        <f t="shared" ref="C27" si="2">IF((D27&lt;&gt;""),ROW(A13),"-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="str">
+        <f>IF((D28&lt;&gt;""),ROW(A14),"-")</f>
+        <v>-</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Oui">
+      <formula>NOT(ISERROR(SEARCH("Oui",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modification planning_projet & suivi_projet
</commit_message>
<xml_diff>
--- a/Gestion projet/planning_projet.xlsx
+++ b/Gestion projet/planning_projet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\stage\Stage_2025_ST_felixDL\Gestion projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A75DF5A-0C7A-4FAF-9923-EBCBA0A81F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E236578-1799-4431-B9F8-DFCD1CD597FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Réalisation du système</t>
   </si>
@@ -101,13 +101,19 @@
     <t>Oui</t>
   </si>
   <si>
-    <t>Information potentiel</t>
-  </si>
-  <si>
     <t>Réaliser le brouillon de l'algorithme</t>
   </si>
   <si>
     <t>Communication entre les appareils</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Visual Studio Code</t>
+  </si>
+  <si>
+    <t>Information potentielle</t>
   </si>
 </sst>
 </file>
@@ -157,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -169,9 +175,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -465,7 +468,7 @@
   <dimension ref="B2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +502,7 @@
         <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -528,6 +531,12 @@
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
@@ -540,6 +549,12 @@
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
@@ -547,7 +562,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>8</v>
@@ -646,10 +661,10 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
-        <f>IF((D16&lt;&gt;""),ROW(A1),"-")</f>
+        <f t="shared" ref="C16:C21" si="2">IF((D16&lt;&gt;""),ROW(A1),"-")</f>
         <v>1</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -658,7 +673,7 @@
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
-        <f>IF((D17&lt;&gt;""),ROW(A2),"-")</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -670,7 +685,7 @@
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
-        <f>IF((D18&lt;&gt;""),ROW(A3),"-")</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -682,7 +697,7 @@
     </row>
     <row r="19" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
-        <f>IF((D19&lt;&gt;""),ROW(A4),"-")</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -694,11 +709,11 @@
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
-        <f>IF((D20&lt;&gt;""),ROW(A5),"-")</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>8</v>
@@ -706,7 +721,7 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="str">
-        <f>IF((D21&lt;&gt;""),ROW(A6),"-")</f>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
@@ -742,7 +757,7 @@
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="str">
-        <f t="shared" ref="C27" si="2">IF((D27&lt;&gt;""),ROW(A13),"-")</f>
+        <f t="shared" ref="C27" si="3">IF((D27&lt;&gt;""),ROW(A13),"-")</f>
         <v>-</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modification fichiers Gestion projet
planning_projet
suivi_projet
</commit_message>
<xml_diff>
--- a/Gestion projet/planning_projet.xlsx
+++ b/Gestion projet/planning_projet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\stage\Stage_2025_ST_felixDL\Gestion projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783EF671-F251-41B4-B834-C1B65FC2E89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D7BA2B-8807-446B-94FE-96689C99EBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="50">
   <si>
     <t>Réalisation du système</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>QtCreator</t>
+  </si>
+  <si>
+    <t>Skipped</t>
   </si>
 </sst>
 </file>
@@ -596,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +743,9 @@
       <c r="F7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -754,7 +759,9 @@
       <c r="F8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -773,7 +780,9 @@
       <c r="F9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -792,7 +801,9 @@
       <c r="F10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -810,7 +821,9 @@
       <c r="F11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -828,7 +841,9 @@
       <c r="F12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -846,7 +861,9 @@
       <c r="F13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -864,7 +881,9 @@
       <c r="F14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -878,7 +897,9 @@
       <c r="F15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -892,7 +913,9 @@
       <c r="F16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -906,7 +929,9 @@
       <c r="F17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -920,7 +945,9 @@
       <c r="F18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -934,7 +961,9 @@
       <c r="F19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -948,7 +977,9 @@
       <c r="F20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="4"/>
+      <c r="G20" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -962,7 +993,9 @@
       <c r="F21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -976,7 +1009,9 @@
       <c r="F22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="4"/>
+      <c r="G22" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1004,7 +1039,9 @@
       <c r="F24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="4"/>
+      <c r="G24" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1032,7 +1069,9 @@
       <c r="F26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modification fichiers Gestion projet + guide installation
Gestion projet = planning et suivi projet
</commit_message>
<xml_diff>
--- a/Gestion projet/planning_projet.xlsx
+++ b/Gestion projet/planning_projet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\stage\Stage_2025_ST_felixDL\Gestion projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D7BA2B-8807-446B-94FE-96689C99EBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905BA777-3B08-4933-BA29-90886DBDD0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
   <si>
     <t>Réalisation du système</t>
   </si>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,7 +1025,9 @@
       <c r="F23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="4"/>
+      <c r="G23" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1055,7 +1057,9 @@
       <c r="F25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modification gestion (oubli du commit d'avant)
</commit_message>
<xml_diff>
--- a/Gestion projet/planning_projet.xlsx
+++ b/Gestion projet/planning_projet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\stage\Stage_2025_ST_felixDL\Gestion projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Stage\Stage_2025_ST_felixDL\Gestion projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905BA777-3B08-4933-BA29-90886DBDD0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020AED13-5BA7-40BB-BA14-DDD424AE2507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
   <si>
     <t>Réalisation du système</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Skipped</t>
+  </si>
+  <si>
+    <t>Implémenter le bouton "Modifier un indice"</t>
   </si>
 </sst>
 </file>
@@ -597,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,7 +1087,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="17"/>
       <c r="E27" s="12" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>6</v>
@@ -1097,8 +1100,8 @@
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
       <c r="D28" s="17"/>
-      <c r="E28" s="8" t="s">
-        <v>39</v>
+      <c r="E28" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>6</v>
@@ -1112,7 +1115,7 @@
       <c r="C29" s="15"/>
       <c r="D29" s="17"/>
       <c r="E29" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>6</v>
@@ -1123,14 +1126,10 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="4">
-        <v>11</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>6</v>
+      <c r="C30" s="15"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>6</v>
@@ -1140,48 +1139,48 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4">
+        <v>11</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="B32" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="4">
+      <c r="C33" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>6</v>
+      <c r="D33" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -1190,10 +1189,10 @@
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>6</v>
@@ -1208,10 +1207,10 @@
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>6</v>
@@ -1222,14 +1221,14 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>6</v>
@@ -1240,14 +1239,14 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>6</v>
@@ -1262,10 +1261,10 @@
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>6</v>
@@ -1280,10 +1279,10 @@
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>6</v>
@@ -1298,10 +1297,10 @@
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>6</v>
@@ -1315,10 +1314,18 @@
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="4"/>
+      <c r="C41" s="4">
+        <v>8</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
@@ -1366,7 +1373,7 @@
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
-      <c r="D46" s="1"/>
+      <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -1396,7 +1403,7 @@
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
-      <c r="D49" s="9"/>
+      <c r="D49" s="1"/>
       <c r="E49" s="9"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -1406,7 +1413,7 @@
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
-      <c r="D50" s="1"/>
+      <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -1416,7 +1423,7 @@
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
-      <c r="D51" s="9"/>
+      <c r="D51" s="1"/>
       <c r="E51" s="9"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -1488,7 +1495,7 @@
       <c r="C58" s="4"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
-      <c r="F58" s="5"/>
+      <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
     </row>
@@ -1508,7 +1515,7 @@
       <c r="C60" s="4"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
-      <c r="F60" s="4"/>
+      <c r="F60" s="5"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
     </row>
@@ -1558,7 +1565,7 @@
       <c r="C65" s="4"/>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
-      <c r="F65" s="5"/>
+      <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
     </row>
@@ -1568,8 +1575,8 @@
       <c r="C66" s="4"/>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="8"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="4"/>
       <c r="H66" s="4"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -1589,7 +1596,7 @@
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
       <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
+      <c r="G68" s="8"/>
       <c r="H68" s="4"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -1612,17 +1619,27 @@
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
     </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C14:C29"/>
-    <mergeCell ref="D14:D29"/>
+    <mergeCell ref="C14:C30"/>
+    <mergeCell ref="D14:D30"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G71:G1048576">
+  <conditionalFormatting sqref="G72:G1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Oui">
-      <formula>NOT(ISERROR(SEARCH("Oui",G71)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Oui",G72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modification planning_projet + ajout PDF test pour aide dans l'application
</commit_message>
<xml_diff>
--- a/Gestion projet/planning_projet.xlsx
+++ b/Gestion projet/planning_projet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Stage\Stage_2025_ST_felixDL\Gestion projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020AED13-5BA7-40BB-BA14-DDD424AE2507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0444EB30-226D-4F99-9C23-C5A7002EB63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="51">
   <si>
     <t>Réalisation du système</t>
   </si>
@@ -603,7 +603,7 @@
   <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1092,9 @@
       <c r="F27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>